<commit_message>
Complete settings of Celery, Redis, Dockerfile and docker-compose.yml; tasks for raports
</commit_message>
<xml_diff>
--- a/media/download/raporty.xlsx
+++ b/media/download/raporty.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,17 +506,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-07-04</t>
+          <t>2023-07-17</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Noll Roman</t>
+          <t>Admin</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Projektowanie aplikacji webowej</t>
+          <t>Test 1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -534,52 +534,40 @@
           <t>8:00</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>00.00</t>
-        </is>
+      <c r="G3" t="n">
+        <v>0</v>
       </c>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>136.0</t>
-        </is>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>50</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>160</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-07-10</t>
+          <t>2023-07-15</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Noll Roman</t>
+          <t>Admin</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Test 6</t>
+          <t>Test 1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -597,148 +585,65 @@
           <t>8:00</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>00.00</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Schlosser</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>10.00</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>136.0</t>
-        </is>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>50</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>160</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2023-07-11</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Noll Roman</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Test 6</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>8:00</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>00.00</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Schlosser</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>20.00</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>136.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>RAZEM:</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>438</v>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>24:0</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
+      <c r="B6" t="n">
+        <v>200</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>16:0</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>0:00</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="n">
-        <v>20</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>10</v>
-      </c>
-      <c r="M7" t="n">
-        <v>408</v>
-      </c>
-      <c r="N7" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>100</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>320</v>
+      </c>
+      <c r="N6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>